<commit_message>
Fix #9722 - [Feature] Translate export search reports
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
@@ -9,18 +9,13 @@
   </bookViews>
   <sheets>
     <sheet name="Eco emballage" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Matériaux" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Materials" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$6</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Matériaux!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -365,19 +360,19 @@
     <t xml:space="preserve">Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Nom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matériaux</t>
+    <t xml:space="preserve">Materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecotax category</t>
   </si>
   <si>
     <t xml:space="preserve">CONCAT</t>
   </si>
   <si>
-    <t xml:space="preserve">Poids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niveau</t>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level</t>
   </si>
 </sst>
 </file>
@@ -388,7 +383,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -441,15 +436,6 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -458,13 +444,6 @@
       <b val="true"/>
       <sz val="8"/>
       <color rgb="FFCCCCCC"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -484,7 +463,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,12 +488,6 @@
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66CCFF"/>
-        <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
@@ -787,10 +760,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
@@ -803,15 +772,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -819,11 +792,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -874,7 +847,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF66CCFF"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -885,7 +858,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF7F7F7F"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004254"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -910,7 +883,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -921,8 +894,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
+          <a:off x="33600600" y="290520"/>
+          <a:ext cx="177840" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1000,7 +973,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -1011,8 +984,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
+          <a:off x="33600600" y="290520"/>
+          <a:ext cx="177840" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1090,7 +1063,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -1101,8 +1074,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
+          <a:off x="33600600" y="290520"/>
+          <a:ext cx="177840" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1180,7 +1153,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
@@ -1191,8 +1164,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33595560" y="290520"/>
-          <a:ext cx="178560" cy="360"/>
+          <a:off x="33600600" y="290520"/>
+          <a:ext cx="177840" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1275,11 +1248,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC9" activeCellId="0" sqref="AC9:AC10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X6" activeCellId="0" sqref="6:6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
@@ -1599,97 +1572,97 @@
       <c r="I6" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="K6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="25" t="s">
+      <c r="N6" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="P6" s="25" t="s">
+      <c r="P6" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="25" t="s">
+      <c r="Q6" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="R6" s="25" t="s">
+      <c r="R6" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="S6" s="25" t="s">
+      <c r="S6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="T6" s="25" t="s">
+      <c r="T6" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="U6" s="25" t="s">
+      <c r="U6" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="V6" s="25" t="s">
+      <c r="V6" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="W6" s="25" t="s">
+      <c r="W6" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="X6" s="25" t="s">
+      <c r="X6" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="Y6" s="25" t="s">
+      <c r="Y6" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="Z6" s="25" t="s">
+      <c r="Z6" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="AA6" s="25" t="s">
+      <c r="AA6" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AB6" s="25" t="s">
+      <c r="AB6" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AC6" s="25" t="s">
+      <c r="AC6" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AD6" s="25" t="s">
+      <c r="AD6" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AE6" s="25" t="s">
+      <c r="AE6" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AF6" s="25" t="s">
+      <c r="AF6" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AG6" s="25" t="s">
+      <c r="AG6" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AH6" s="25" t="s">
+      <c r="AH6" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AI6" s="25" t="s">
+      <c r="AI6" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AJ6" s="25" t="s">
+      <c r="AJ6" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="AK6" s="25" t="s">
+      <c r="AK6" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="AL6" s="25" t="s">
+      <c r="AL6" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AM6" s="25" t="s">
+      <c r="AM6" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="AN6" s="26" t="s">
+      <c r="AN6" s="25" t="s">
         <v>83</v>
       </c>
       <c r="AME6" s="13"/>
@@ -1697,7 +1670,7 @@
       <c r="AMG6" s="13"/>
       <c r="AMH6" s="13"/>
       <c r="AMI6" s="13"/>
-      <c r="AMJ6" s="14"/>
+      <c r="AMJ6" s="26"/>
     </row>
     <row r="7" s="27" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="27" t="s">
@@ -1839,14 +1812,14 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="AC9:AC10 F1"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="6:6 I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1896,13 +1869,13 @@
         <v>103</v>
       </c>
       <c r="C3" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="E3" s="32" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>84</v>
       </c>
       <c r="F3" s="32" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Fix #12728 - [Bug] Fix citeo en report
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
@@ -12,10 +12,8 @@
     <sheet name="Materials" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$6</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Eco emballage'!$A$6:$AE$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -143,7 +141,7 @@
     <t xml:space="preserve">Product</t>
   </si>
   <si>
-    <t xml:space="preserve">Materials weights</t>
+    <t xml:space="preserve">Materials weight</t>
   </si>
   <si>
     <t xml:space="preserve">Rebate</t>
@@ -219,7 +217,10 @@
     <t xml:space="preserve">Aluminium</t>
   </si>
   <si>
-    <t xml:space="preserve">Brick</t>
+    <t xml:space="preserve">Paper and cardboard other than bricks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bricks</t>
   </si>
   <si>
     <t xml:space="preserve">Glass</t>
@@ -298,42 +299,6 @@
   </si>
   <si>
     <t xml:space="preserve">Total per line</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catégorie ecotaxe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 .6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.3</t>
   </si>
   <si>
     <t xml:space="preserve">pack:packMaterialList</t>
@@ -443,7 +408,7 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
-      <color rgb="FFCCCCCC"/>
+      <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -463,7 +428,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,24 +437,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF004254"/>
-        <bgColor rgb="FF003300"/>
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009FE3"/>
+        <bgColor rgb="FF00B2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2987A"/>
+        <bgColor rgb="FFED7483"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DC799"/>
+        <bgColor rgb="FFA7D2AE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7483"/>
+        <bgColor rgb="FFF2987A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B2CC"/>
+        <bgColor rgb="FF009FE3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFF7C7CD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FF80CEF4"/>
+        <bgColor rgb="FF8DC799"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDD17A"/>
+        <bgColor rgb="FFF7C7CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA7D2AE"/>
+        <bgColor rgb="FF8DC799"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7C7CD"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF004254"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -521,80 +540,8 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color rgb="FFF2F2F2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="thin">
         <color rgb="FFFFFFFF"/>
       </right>
@@ -630,17 +577,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -667,7 +603,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -684,7 +620,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -692,111 +628,63 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="true"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -824,15 +712,15 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF009FE3"/>
+      <rgbColor rgb="FFA7D2AE"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF2F2F2"/>
-      <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFF7C7CD"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFED7483"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
@@ -843,14 +731,14 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FF00B2CC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FF80CEF4"/>
+      <rgbColor rgb="FFF2987A"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFDD17A"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -858,7 +746,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF8DC799"/>
       <rgbColor rgb="FF004254"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -876,26 +764,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>245880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>389520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33600600" y="290520"/>
-          <a:ext cx="177840" cy="360"/>
+          <a:off x="27880920" y="527400"/>
+          <a:ext cx="143640" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -956,7 +844,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -966,26 +854,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>245880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>389520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="1" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33600600" y="290520"/>
-          <a:ext cx="177840" cy="360"/>
+          <a:off x="27880920" y="527400"/>
+          <a:ext cx="143640" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1046,7 +934,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1056,26 +944,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>245880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>389520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33600600" y="290520"/>
-          <a:ext cx="177840" cy="360"/>
+          <a:off x="27880920" y="527400"/>
+          <a:ext cx="143640" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1136,7 +1024,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1146,26 +1034,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>725040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>245880</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>389520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33600600" y="290520"/>
-          <a:ext cx="177840" cy="360"/>
+          <a:off x="27880920" y="527400"/>
+          <a:ext cx="143640" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1226,7 +1114,7 @@
             </a:rPr>
             <a:t>Suivant</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="fr-FR" sz="1100" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1246,35 +1134,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="A1:AN6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X6" activeCellId="0" sqref="6:6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK19" activeCellId="0" sqref="AK19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="17" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="26" style="0" width="22.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="16.07"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1152,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1373,7 +1241,7 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="2"/>
     </row>
-    <row r="3" s="4" customFormat="true" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -1414,34 +1282,26 @@
         <v>34</v>
       </c>
       <c r="AD3" s="8"/>
-      <c r="AE3" s="9" t="s">
+      <c r="AE3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="10" t="s">
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="11" t="s">
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AK3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AME3" s="13"/>
-      <c r="AMF3" s="13"/>
-      <c r="AMG3" s="13"/>
-      <c r="AMH3" s="13"/>
-      <c r="AMI3" s="13"/>
-      <c r="AMJ3" s="14"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
     </row>
-    <row r="4" s="13" customFormat="true" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>30</v>
       </c>
@@ -1454,41 +1314,40 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18" t="s">
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="17"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="12"/>
-      <c r="AL4" s="12"/>
-      <c r="AM4" s="12"/>
-      <c r="AN4" s="12"/>
-      <c r="AMJ4" s="14"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
     </row>
-    <row r="5" s="14" customFormat="true" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -1501,251 +1360,172 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="10" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="7" t="s">
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7" t="s">
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="10" t="s">
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10" t="s">
+      <c r="W5" s="11"/>
+      <c r="X5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="Y5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
       <c r="AB5" s="7"/>
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AL5" s="12"/>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
     </row>
-    <row r="6" s="21" customFormat="true" ht="65.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
+    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="M6" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="N6" s="24" t="s">
+      <c r="M6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="23" t="s">
+      <c r="N6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="O6" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="24" t="s">
+      <c r="P6" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="R6" s="24" t="s">
+      <c r="Q6" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="S6" s="24" t="s">
+      <c r="R6" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="T6" s="24" t="s">
+      <c r="S6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="U6" s="24" t="s">
+      <c r="T6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="V6" s="24" t="s">
+      <c r="U6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="W6" s="24" t="s">
+      <c r="V6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="X6" s="24" t="s">
+      <c r="W6" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="Y6" s="24" t="s">
+      <c r="X6" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="Z6" s="24" t="s">
+      <c r="Y6" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AA6" s="24" t="s">
+      <c r="Z6" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AB6" s="24" t="s">
+      <c r="AA6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AC6" s="24" t="s">
+      <c r="AB6" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="AD6" s="24" t="s">
+      <c r="AC6" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="AE6" s="24" t="s">
+      <c r="AD6" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="AF6" s="24" t="s">
+      <c r="AE6" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="AG6" s="24" t="s">
+      <c r="AF6" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="AH6" s="24" t="s">
+      <c r="AG6" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="AI6" s="24" t="s">
+      <c r="AH6" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="AJ6" s="24" t="s">
+      <c r="AI6" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="AK6" s="24" t="s">
+      <c r="AJ6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="AL6" s="24" t="s">
+      <c r="AK6" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="AM6" s="24" t="s">
+      <c r="AL6" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="AN6" s="25" t="s">
+      <c r="AM6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="AME6" s="13"/>
-      <c r="AMF6" s="13"/>
-      <c r="AMG6" s="13"/>
-      <c r="AMH6" s="13"/>
-      <c r="AMI6" s="13"/>
-      <c r="AMJ6" s="26"/>
-    </row>
-    <row r="7" s="27" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="28" t="s">
+      <c r="AN6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="N7" s="29" t="n">
-        <v>4</v>
-      </c>
-      <c r="O7" s="29" t="n">
-        <v>5</v>
-      </c>
-      <c r="P7" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q7" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="R7" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="S7" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="T7" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="U7" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="V7" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="W7" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="X7" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y7" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z7" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA7" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="0"/>
-      <c r="AD7" s="0"/>
-      <c r="AE7" s="0"/>
-      <c r="AMJ7" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A6:AE6"/>
   <mergeCells count="15">
     <mergeCell ref="B3:J5"/>
     <mergeCell ref="K3:AA3"/>
@@ -1755,47 +1535,35 @@
     <mergeCell ref="AG3:AI5"/>
     <mergeCell ref="AJ3:AJ5"/>
     <mergeCell ref="AK3:AN5"/>
-    <mergeCell ref="P4:X4"/>
+    <mergeCell ref="K4:AA4"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="P5:R5"/>
     <mergeCell ref="S5:U5"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="Y5:AA5"/>
-    <mergeCell ref="B7:J7"/>
   </mergeCells>
-  <dataValidations count="7">
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AN3" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" prompt="Indiquez OUI si votre emballage est en papier-carton recyclé et qu'il contient plus de 50% de recyclé. &#10;Sinon, laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AB6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place :&#10;- Consigne 8% (On-pack/notice)&#10;- Off-Pack 4%&#10;- Consigne + Off-Pack 12%&#10;- Triman uniquement 5%&#10;- Triman + off-pack 9%&#10;Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC6" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place :&#10;- Consigne 8% (On-pack/notice)&#10;- Off-Pack 4%&#10;- Consigne + Off-Pack 12%&#10;- Triman uniquement 5%&#10;- Triman + off-pack 9%&#10;Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AC6:AF6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action mise en place :&#10;- Réduction de poids 8%&#10;- Suppression d’une unité 8%&#10;Sinon, laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AD6" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place :&#10;- Consigne 8% (On-pack/notice)&#10;- QR code 4%&#10;- Off-Pack 4%&#10;- Consigne + Off-Pack 12%&#10;- QR Code + Off-Pack 8%&#10;- Triman uniquement 5%&#10;- Triman + Off-Pack 9%&#10;Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AE6 AG6" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Choisissez dans la liste déroulante.&#10;Sinon laissez la case vide.&#10;" promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AH6:AI6" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le nombre d'Unités de Vente Consommateur (UVC) mises sur le marché français." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AJ6" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AN3" type="none">
+    <dataValidation allowBlank="true" operator="between" prompt="Indiquez le type d'action de sensibilisation mise en place :&#10;- Consigne 8% (On-pack/notice)&#10;- QR code 4%&#10;- Off-Pack 4%&#10;- Consigne + Off-Pack 12%&#10;- QR Code + Off-Pack 8%&#10;- Triman uniquement 5%&#10;- Triman + Off-Pack 9%&#10;Sinon laissez la case vide." promptTitle="Aide à la saisie :" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="AG6:AI6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1812,10 +1580,10 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="1" sqref="6:6 I2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
@@ -1828,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -1843,52 +1611,52 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>100</v>
+        <v>86</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>108</v>
+      <c r="D3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H3"/>
+  <autoFilter ref="B3:H4"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Fix #12728 - [Bug] Update ExportCiteo.xlsx
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
@@ -12,8 +12,8 @@
     <sheet name="Materials" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -81,55 +81,55 @@
     <t xml:space="preserve">formula|""</t>
   </si>
   <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("K"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("L"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("M"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("N"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("O"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("P"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("Q"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("R"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("S"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("T"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("U"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("V"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("W"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("X"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("Y"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("Z"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("AA"&amp;ROW($A$2)+5)&amp;"P",Matériaux!$F$4:$G$10000,2,FALSE)),"")</t>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("K"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("L"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("M"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("N"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("O"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("P"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("Q"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("R"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("S"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("T"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("U"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("V"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("W"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("X"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("Y"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("Z"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel|IFERROR(IF(G2="","",VLOOKUP(E2&amp;"C"&amp;INDIRECT("AA"&amp;ROW($A$2)+5)&amp;"P",Materials!$F$4:$G$10000,2,FALSE)),"")</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:labelClaimList[bcpg:lclLabelClaim#bcpg:labelClaimCode=="ECO\\_PACK\\_50\\_RECYCLED"]_bcpg:lclClaimValue</t>
@@ -171,10 +171,10 @@
     <t xml:space="preserve">Bottle</t>
   </si>
   <si>
-    <t xml:space="preserve">Hard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thin</t>
+    <t xml:space="preserve">Rigid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flexible</t>
   </si>
   <si>
     <t xml:space="preserve">PVC</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">Aluminium</t>
   </si>
   <si>
-    <t xml:space="preserve">Paper and cardboard other than bricks</t>
+    <t xml:space="preserve">Paper -cardboard other than bricks</t>
   </si>
   <si>
     <t xml:space="preserve">Bricks</t>
@@ -226,31 +226,31 @@
     <t xml:space="preserve">Glass</t>
   </si>
   <si>
-    <t xml:space="preserve">Clear PET bottles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dark PET bottles</t>
+    <t xml:space="preserve">Clear PET Bottle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark/colored PET, PE, PP Bottle</t>
   </si>
   <si>
     <t xml:space="preserve">Other bottles (not PVC)</t>
   </si>
   <si>
-    <t xml:space="preserve">Hard packaging  in PP, PE or PET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hard packaging in PS</t>
+    <t xml:space="preserve">Rigid packaging PE, PP or PET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rigid PS packaging</t>
   </si>
   <si>
     <t xml:space="preserve">Other packaging (not PVC)</t>
   </si>
   <si>
-    <t xml:space="preserve">Thin PE packaging</t>
+    <t xml:space="preserve">Flexible PE packaging</t>
   </si>
   <si>
     <t xml:space="preserve">Other thin packaging</t>
   </si>
   <si>
-    <t xml:space="preserve">PVC based packaging</t>
+    <t xml:space="preserve">Packaging containing PVC</t>
   </si>
   <si>
     <t xml:space="preserve">Raw wood and cork</t>
@@ -771,7 +771,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389520</xdr:colOff>
+      <xdr:colOff>389160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
@@ -782,8 +782,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27880920" y="527400"/>
-          <a:ext cx="143640" cy="360"/>
+          <a:off x="27924120" y="527400"/>
+          <a:ext cx="143280" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -861,7 +861,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389520</xdr:colOff>
+      <xdr:colOff>389160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
@@ -872,8 +872,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27880920" y="527400"/>
-          <a:ext cx="143640" cy="360"/>
+          <a:off x="27924120" y="527400"/>
+          <a:ext cx="143280" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -951,7 +951,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389520</xdr:colOff>
+      <xdr:colOff>389160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
@@ -962,8 +962,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27880920" y="527400"/>
-          <a:ext cx="143640" cy="360"/>
+          <a:off x="27924120" y="527400"/>
+          <a:ext cx="143280" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1041,7 +1041,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389520</xdr:colOff>
+      <xdr:colOff>389160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
@@ -1052,8 +1052,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27880920" y="527400"/>
-          <a:ext cx="143640" cy="360"/>
+          <a:off x="27924120" y="527400"/>
+          <a:ext cx="143280" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1136,11 +1136,11 @@
   </sheetPr>
   <dimension ref="A1:AN6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK19" activeCellId="0" sqref="AK19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S6" activeCellId="0" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1580,10 +1580,10 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="U21" activeCellId="0" sqref="U21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
@@ -1656,7 +1656,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H4"/>
+  <autoFilter ref="B3:H3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Fix #12728 - [Bug] Update Citeo export report file
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportCiteo.xlsx
@@ -12,8 +12,8 @@
     <sheet name="Materials" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Materials!$B$3:$H$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -186,13 +186,13 @@
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Commercial label</t>
+    <t xml:space="preserve">Trade name</t>
   </si>
   <si>
     <t xml:space="preserve">Label</t>
   </si>
   <si>
-    <t xml:space="preserve">BeCPG Code</t>
+    <t xml:space="preserve">beCPG Code</t>
   </si>
   <si>
     <t xml:space="preserve">ERP Code</t>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">Product Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Legal label</t>
+    <t xml:space="preserve">Legal name</t>
   </si>
   <si>
     <t xml:space="preserve">Number of packaging units on the product
@@ -299,6 +299,39 @@
   </si>
   <si>
     <t xml:space="preserve">Total per line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 .6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.3</t>
   </si>
   <si>
     <t xml:space="preserve">pack:packMaterialList</t>
@@ -428,7 +461,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,7 +507,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFF7C7CD"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -499,6 +532,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF7C7CD"/>
         <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -603,7 +642,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -676,15 +715,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="true"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -717,7 +760,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF7C7CD"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFED7483"/>
@@ -737,7 +780,7 @@
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF80CEF4"/>
       <rgbColor rgb="FFF2987A"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFF7C7CD"/>
       <rgbColor rgb="FFFDD17A"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -767,13 +810,13 @@
       <xdr:col>34</xdr:col>
       <xdr:colOff>245880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389160</xdr:colOff>
+      <xdr:colOff>388080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -782,8 +825,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27924120" y="527400"/>
-          <a:ext cx="143280" cy="360"/>
+          <a:off x="28053720" y="527760"/>
+          <a:ext cx="142200" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -857,13 +900,13 @@
       <xdr:col>34</xdr:col>
       <xdr:colOff>245880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389160</xdr:colOff>
+      <xdr:colOff>388080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -872,8 +915,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27924120" y="527400"/>
-          <a:ext cx="143280" cy="360"/>
+          <a:off x="28053720" y="527760"/>
+          <a:ext cx="142200" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -947,13 +990,13 @@
       <xdr:col>34</xdr:col>
       <xdr:colOff>245880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389160</xdr:colOff>
+      <xdr:colOff>388080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -962,8 +1005,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27924120" y="527400"/>
-          <a:ext cx="143280" cy="360"/>
+          <a:off x="28053720" y="527760"/>
+          <a:ext cx="142200" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1037,13 +1080,13 @@
       <xdr:col>34</xdr:col>
       <xdr:colOff>245880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>389160</xdr:colOff>
+      <xdr:colOff>388080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>62640</xdr:rowOff>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1052,8 +1095,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27924120" y="527400"/>
-          <a:ext cx="143280" cy="360"/>
+          <a:off x="28053720" y="527760"/>
+          <a:ext cx="142200" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst>
@@ -1134,13 +1177,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AN7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S6" activeCellId="0" sqref="S6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1523,6 +1566,62 @@
       </c>
       <c r="AN6" s="13" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" s="18" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="O7" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q7" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="R7" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="V7" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="W7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y7" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z7" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA7" s="18" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1583,12 +1682,12 @@
       <selection pane="topLeft" activeCell="U21" activeCellId="0" sqref="U21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,12 +1695,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -1611,52 +1706,52 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>89</v>
+        <v>97</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>91</v>
+        <v>101</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>97</v>
+      <c r="D3" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H3"/>
+  <autoFilter ref="B3:H4"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>